<commit_message>
Final comments and organizational stuff
</commit_message>
<xml_diff>
--- a/Cleaned_data.xlsx
+++ b/Cleaned_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessebecklevisohn/Documents/GitHub/group3-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessebecklevisohn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8762C8F-F916-F340-947B-ABF9FEF85D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA03CF3-24A2-0A4E-97EF-540600967E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pH control" sheetId="16" r:id="rId1"/>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E56E3F-1479-4A01-BE4B-B82BF68EA56D}">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6405,8 +6405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71BF8D5C-9BDE-4ECA-9270-5B09D81E1D28}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6458,7 +6458,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -6479,8 +6479,8 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f xml:space="preserve"> MOD(I2 + 1, 10) + 10</f>
-        <v>11</v>
+        <f xml:space="preserve"> MOD(I2 + 1, 10)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -6501,8 +6501,8 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I41" si="1" xml:space="preserve"> MOD(I3 + 1, 10) + 10</f>
-        <v>12</v>
+        <f t="shared" ref="I4:I41" si="1" xml:space="preserve"> MOD(I3 + 1, 10)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -6524,7 +6524,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -6546,7 +6546,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -6568,7 +6568,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -6590,7 +6590,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -6612,7 +6612,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -6634,7 +6634,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -6656,7 +6656,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -6687,7 +6687,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -6718,7 +6718,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -6749,7 +6749,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -6780,7 +6780,7 @@
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -6811,7 +6811,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -6842,7 +6842,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -6873,7 +6873,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -6904,7 +6904,7 @@
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -6935,7 +6935,7 @@
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -6966,7 +6966,7 @@
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -6997,7 +6997,7 @@
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -7090,7 +7090,7 @@
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -7121,7 +7121,7 @@
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -7152,7 +7152,7 @@
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -7183,7 +7183,7 @@
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -7214,7 +7214,7 @@
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -7245,7 +7245,7 @@
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -7276,7 +7276,7 @@
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -7307,7 +7307,7 @@
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -7338,7 +7338,7 @@
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -7369,7 +7369,7 @@
       </c>
       <c r="I34">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -7400,7 +7400,7 @@
       </c>
       <c r="I35">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -7431,7 +7431,7 @@
       </c>
       <c r="I36">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -7462,7 +7462,7 @@
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -7493,7 +7493,7 @@
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -7524,7 +7524,7 @@
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -7555,7 +7555,7 @@
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -7586,7 +7586,7 @@
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -8755,8 +8755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D33F4DE-1FD6-1249-AAB3-117BF50CF73F}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8811,7 +8811,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -8831,8 +8831,8 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f xml:space="preserve"> MOD(I2 + 1, 10) + 10</f>
-        <v>11</v>
+        <f xml:space="preserve"> MOD(I2 + 1, 10)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -8852,8 +8852,8 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I41" si="0" xml:space="preserve"> MOD(I3 + 1, 10) + 10</f>
-        <v>12</v>
+        <f t="shared" ref="I4:I41" si="0" xml:space="preserve"> MOD(I3 + 1, 10)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -8874,7 +8874,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -8895,7 +8895,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -8916,7 +8916,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -8937,7 +8937,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -8958,7 +8958,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -8979,7 +8979,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -9000,7 +9000,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -9030,7 +9030,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -9060,7 +9060,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -9090,7 +9090,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -9120,7 +9120,7 @@
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -9150,7 +9150,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -9180,7 +9180,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -9210,7 +9210,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -9240,7 +9240,7 @@
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -9270,7 +9270,7 @@
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -9300,7 +9300,7 @@
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -9330,7 +9330,7 @@
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -9360,7 +9360,7 @@
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -9390,7 +9390,7 @@
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -9420,7 +9420,7 @@
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -9450,7 +9450,7 @@
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -9480,7 +9480,7 @@
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -9510,7 +9510,7 @@
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -9540,7 +9540,7 @@
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -9570,7 +9570,7 @@
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -9600,7 +9600,7 @@
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -9630,7 +9630,7 @@
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -9660,7 +9660,7 @@
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -9690,7 +9690,7 @@
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -9720,7 +9720,7 @@
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -9750,7 +9750,7 @@
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -9780,7 +9780,7 @@
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -9810,7 +9810,7 @@
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -9840,7 +9840,7 @@
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -9870,7 +9870,7 @@
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -9900,7 +9900,7 @@
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -9912,8 +9912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27F87D8-61D0-DF4D-A010-96854C67E199}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9968,7 +9968,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -9988,8 +9988,8 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f xml:space="preserve"> MOD(I2 + 1, 10) + 10</f>
-        <v>11</v>
+        <f xml:space="preserve"> MOD(I2 + 1, 10)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -10009,8 +10009,8 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I41" si="0" xml:space="preserve"> MOD(I3 + 1, 10) + 10</f>
-        <v>12</v>
+        <f t="shared" ref="I4:I41" si="0" xml:space="preserve"> MOD(I3 + 1, 10)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -10031,7 +10031,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -10052,7 +10052,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -10073,7 +10073,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -10094,7 +10094,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -10115,7 +10115,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -10136,7 +10136,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -10157,7 +10157,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -10188,7 +10188,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -10219,7 +10219,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -10250,7 +10250,7 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -10281,7 +10281,7 @@
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -10312,7 +10312,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -10343,7 +10343,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -10374,7 +10374,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -10405,7 +10405,7 @@
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -10436,7 +10436,7 @@
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -10467,7 +10467,7 @@
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -10498,7 +10498,7 @@
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -10529,7 +10529,7 @@
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -10560,7 +10560,7 @@
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -10591,7 +10591,7 @@
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -10622,7 +10622,7 @@
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -10653,7 +10653,7 @@
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -10684,7 +10684,7 @@
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -10715,7 +10715,7 @@
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -10746,7 +10746,7 @@
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -10777,7 +10777,7 @@
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -10808,7 +10808,7 @@
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -10839,7 +10839,7 @@
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -10870,7 +10870,7 @@
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -10901,7 +10901,7 @@
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -10932,7 +10932,7 @@
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -10994,7 +10994,7 @@
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -11025,7 +11025,7 @@
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -11056,7 +11056,7 @@
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -11099,8 +11099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20815BDD-EA8C-2D46-845A-59FD9781CE26}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>